<commit_message>
Updated data for new month.
</commit_message>
<xml_diff>
--- a/input/Docks_Consumption_AbsPlusNorm.xlsx
+++ b/input/Docks_Consumption_AbsPlusNorm.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16935" tabRatio="693"/>
   </bookViews>
   <sheets>
-    <sheet name="11_2016" sheetId="12" r:id="rId1"/>
-    <sheet name="10_2016" sheetId="2" r:id="rId2"/>
-    <sheet name="9_2016" sheetId="4" r:id="rId3"/>
-    <sheet name="8_2016" sheetId="5" r:id="rId4"/>
-    <sheet name="7_2016" sheetId="6" r:id="rId5"/>
-    <sheet name="6_2016" sheetId="7" r:id="rId6"/>
-    <sheet name="5_2016" sheetId="8" r:id="rId7"/>
-    <sheet name="4_2016" sheetId="9" r:id="rId8"/>
-    <sheet name="3_2016" sheetId="10" r:id="rId9"/>
-    <sheet name="2_2016" sheetId="3" r:id="rId10"/>
-    <sheet name="1_2016" sheetId="1" r:id="rId11"/>
-    <sheet name="12_2015" sheetId="11" r:id="rId12"/>
+    <sheet name="12_2016" sheetId="11" r:id="rId1"/>
+    <sheet name="11_2016" sheetId="12" r:id="rId2"/>
+    <sheet name="10_2016" sheetId="2" r:id="rId3"/>
+    <sheet name="9_2016" sheetId="4" r:id="rId4"/>
+    <sheet name="8_2016" sheetId="5" r:id="rId5"/>
+    <sheet name="7_2016" sheetId="6" r:id="rId6"/>
+    <sheet name="6_2016" sheetId="7" r:id="rId7"/>
+    <sheet name="5_2016" sheetId="8" r:id="rId8"/>
+    <sheet name="4_2016" sheetId="9" r:id="rId9"/>
+    <sheet name="3_2016" sheetId="10" r:id="rId10"/>
+    <sheet name="2_2016" sheetId="3" r:id="rId11"/>
+    <sheet name="1_2016" sheetId="1" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -447,15 +447,10 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -503,28 +498,28 @@
         <v>2695</v>
       </c>
       <c r="D2" s="2">
-        <v>7598</v>
+        <v>9797</v>
       </c>
       <c r="E2" s="2">
-        <v>2819.294990723562</v>
+        <v>3635.2504638218925</v>
       </c>
       <c r="F2" s="2">
-        <v>222.61772486772483</v>
+        <v>220.42804232804232</v>
       </c>
       <c r="G2" s="2">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H2" s="2">
-        <v>95.407596371882065</v>
+        <v>99.032888582163935</v>
       </c>
       <c r="I2" s="2">
-        <v>130.71428571428572</v>
+        <v>135.68115942028984</v>
       </c>
       <c r="J2" s="2">
-        <v>134.75</v>
+        <v>188.64999999999998</v>
       </c>
       <c r="K2" s="2">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -538,28 +533,28 @@
         <v>3100</v>
       </c>
       <c r="D3" s="2">
-        <v>8496</v>
+        <v>10697</v>
       </c>
       <c r="E3" s="2">
-        <v>2740.6451612903224</v>
+        <v>3450.6451612903224</v>
       </c>
       <c r="F3" s="2">
-        <v>364.53233151183974</v>
+        <v>374.61156648451731</v>
       </c>
       <c r="G3" s="2">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="H3" s="2">
-        <v>156.22814207650276</v>
+        <v>168.30374726115997</v>
       </c>
       <c r="I3" s="2">
-        <v>151</v>
+        <v>200.37681159420291</v>
       </c>
       <c r="J3" s="2">
-        <v>116.25</v>
+        <v>124</v>
       </c>
       <c r="K3" s="2">
-        <v>37.5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -573,28 +568,28 @@
         <v>2800</v>
       </c>
       <c r="D4" s="2">
-        <v>7885</v>
+        <v>10069</v>
       </c>
       <c r="E4" s="2">
-        <v>2816.0714285714284</v>
+        <v>3596.0714285714284</v>
       </c>
       <c r="F4" s="2">
-        <v>306.43223905723903</v>
+        <v>304.83207070707073</v>
       </c>
       <c r="G4" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H4" s="2">
-        <v>131.32810245310245</v>
+        <v>136.95353901332163</v>
       </c>
       <c r="I4" s="2">
-        <v>164.14285714285714</v>
+        <v>171.17391304347825</v>
       </c>
       <c r="J4" s="2">
-        <v>113.39999999999999</v>
+        <v>136.07999999999998</v>
       </c>
       <c r="K4" s="2">
-        <v>40.5</v>
+        <v>48.6</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -608,28 +603,28 @@
         <v>6150</v>
       </c>
       <c r="D5" s="2">
-        <v>17696</v>
+        <v>21938</v>
       </c>
       <c r="E5" s="2">
-        <v>2877.3983739837399</v>
+        <v>3567.1544715447153</v>
       </c>
       <c r="F5" s="2">
-        <v>407.4943310657597</v>
+        <v>408.93424036281175</v>
       </c>
       <c r="G5" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H5" s="2">
-        <v>174.64042759961129</v>
+        <v>183.72407900358209</v>
       </c>
       <c r="I5" s="2">
-        <v>121.28571428571429</v>
+        <v>127.59420289855072</v>
       </c>
       <c r="J5" s="2">
-        <v>169.43249999999998</v>
+        <v>204.48749999999998</v>
       </c>
       <c r="K5" s="2">
-        <v>27.549999999999997</v>
+        <v>33.25</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -643,28 +638,28 @@
         <v>6430</v>
       </c>
       <c r="D6" s="2">
-        <v>18769</v>
+        <v>21903</v>
       </c>
       <c r="E6" s="2">
-        <v>2918.9735614307933</v>
+        <v>3406.3763608087093</v>
       </c>
       <c r="F6" s="2">
-        <v>449.98651564185542</v>
+        <v>447.00647249190939</v>
       </c>
       <c r="G6" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H6" s="2">
-        <v>192.85136384650946</v>
+        <v>200.82899488766944</v>
       </c>
       <c r="I6" s="2">
-        <v>129.42857142857142</v>
+        <v>134.78260869565219</v>
       </c>
       <c r="J6" s="2">
-        <v>279.70499999999998</v>
+        <v>322.14300000000003</v>
       </c>
       <c r="K6" s="2">
-        <v>43.5</v>
+        <v>50.1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -678,28 +673,28 @@
         <v>6435</v>
       </c>
       <c r="D7" s="2">
-        <v>19002</v>
+        <v>22231</v>
       </c>
       <c r="E7" s="2">
-        <v>2952.9137529137529</v>
+        <v>3454.7008547008545</v>
       </c>
       <c r="F7" s="2">
-        <v>341.44415204678364</v>
+        <v>347.74385964912284</v>
       </c>
       <c r="G7" s="2">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="H7" s="2">
-        <v>146.33320802005014</v>
+        <v>156.23274853801172</v>
       </c>
       <c r="I7" s="2">
-        <v>116.14285714285714</v>
+        <v>124</v>
       </c>
       <c r="J7" s="2">
-        <v>225.22500000000002</v>
+        <v>281.53125</v>
       </c>
       <c r="K7" s="2">
-        <v>35</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -713,28 +708,28 @@
         <v>5890</v>
       </c>
       <c r="D8" s="2">
-        <v>17059</v>
+        <v>21498</v>
       </c>
       <c r="E8" s="2">
-        <v>2896.2648556876061</v>
+        <v>3649.9151103565364</v>
       </c>
       <c r="F8" s="2">
-        <v>390.31677890011224</v>
+        <v>388.95679012345681</v>
       </c>
       <c r="G8" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H8" s="2">
-        <v>167.27861952861952</v>
+        <v>174.74870280908928</v>
       </c>
       <c r="I8" s="2">
-        <v>123</v>
+        <v>128.49275362318841</v>
       </c>
       <c r="J8" s="2">
-        <v>189.65800000000002</v>
+        <v>237.07249999999999</v>
       </c>
       <c r="K8" s="2">
-        <v>32.200000000000003</v>
+        <v>40.25</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -748,28 +743,28 @@
         <v>4980</v>
       </c>
       <c r="D9" s="2">
-        <v>15074</v>
+        <v>18898</v>
       </c>
       <c r="E9" s="2">
-        <v>3026.9076305220883</v>
+        <v>3794.7791164658634</v>
       </c>
       <c r="F9" s="2">
-        <v>334.61798679867985</v>
+        <v>333.46809680968096</v>
       </c>
       <c r="G9" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H9" s="2">
-        <v>143.40770862800565</v>
+        <v>149.8190000159436</v>
       </c>
       <c r="I9" s="2">
-        <v>124.71428571428571</v>
+        <v>130.28985507246378</v>
       </c>
       <c r="J9" s="2">
-        <v>259.70699999999999</v>
+        <v>311.99700000000001</v>
       </c>
       <c r="K9" s="2">
-        <v>52.15</v>
+        <v>62.65</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -783,10 +778,10 @@
         <v>7020</v>
       </c>
       <c r="D10" s="2">
-        <v>20629</v>
+        <v>23210</v>
       </c>
       <c r="E10" s="2">
-        <v>2938.6039886039885</v>
+        <v>3306.2678062678065</v>
       </c>
       <c r="F10" s="2">
         <v>678.68</v>
@@ -795,16 +790,16 @@
         <v>361</v>
       </c>
       <c r="H10" s="2">
-        <v>290.86285714285714</v>
+        <v>304.91420289855068</v>
       </c>
       <c r="I10" s="2">
-        <v>154.71428571428572</v>
+        <v>162.18840579710144</v>
       </c>
       <c r="J10" s="2">
-        <v>285.012</v>
+        <v>335.90699999999998</v>
       </c>
       <c r="K10" s="2">
-        <v>40.6</v>
+        <v>47.85</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -818,28 +813,28 @@
         <v>5320</v>
       </c>
       <c r="D11" s="2">
-        <v>15249</v>
+        <v>19503</v>
       </c>
       <c r="E11" s="2">
-        <v>2866.3533834586465</v>
+        <v>3665.9774436090224</v>
       </c>
       <c r="F11" s="2">
-        <v>327.5679012345679</v>
+        <v>325.04814814814813</v>
       </c>
       <c r="G11" s="2">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H11" s="2">
-        <v>140.38624338624336</v>
+        <v>146.03612453032744</v>
       </c>
       <c r="I11" s="2">
-        <v>111.42857142857143</v>
+        <v>115.91304347826087</v>
       </c>
       <c r="J11" s="2">
-        <v>201.39392000000001</v>
+        <v>260.68</v>
       </c>
       <c r="K11" s="2">
-        <v>37.856000000000002</v>
+        <v>49.000000000000007</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -853,28 +848,28 @@
         <v>3570</v>
       </c>
       <c r="D12" s="2">
-        <v>15514</v>
+        <v>17396</v>
       </c>
       <c r="E12" s="2">
-        <v>4345.6582633053222</v>
+        <v>4872.8291316526611</v>
       </c>
       <c r="F12" s="2">
-        <v>219.34649910233392</v>
+        <v>222.87013764213046</v>
       </c>
       <c r="G12" s="2">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="H12" s="2">
-        <v>94.005642472428832</v>
+        <v>100.13006183921803</v>
       </c>
       <c r="I12" s="2">
-        <v>106.71428571428571</v>
+        <v>113.66666666666667</v>
       </c>
       <c r="J12" s="2">
-        <v>130.03200000000001</v>
+        <v>166.25519999999997</v>
       </c>
       <c r="K12" s="2">
-        <v>33.6</v>
+        <v>42.96</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -888,28 +883,28 @@
         <v>7356</v>
       </c>
       <c r="D13" s="2">
-        <v>21231</v>
+        <v>23985</v>
       </c>
       <c r="E13" s="2">
-        <v>2886.2153344208809</v>
+        <v>3260.6035889070145</v>
       </c>
       <c r="F13" s="2">
-        <v>463.01795580110496</v>
+        <v>467.04419889502765</v>
       </c>
       <c r="G13" s="2">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H13" s="2">
-        <v>198.43626677190213</v>
+        <v>209.8314516774762</v>
       </c>
       <c r="I13" s="2">
-        <v>98.571428571428569</v>
+        <v>104.23188405797102</v>
       </c>
       <c r="J13" s="2">
-        <v>213.17688000000001</v>
+        <v>247.16159999999999</v>
       </c>
       <c r="K13" s="2">
-        <v>28.980000000000004</v>
+        <v>33.6</v>
       </c>
     </row>
   </sheetData>
@@ -974,28 +969,28 @@
         <v>2695</v>
       </c>
       <c r="D2" s="2">
-        <v>10159</v>
+        <v>8597</v>
       </c>
       <c r="E2" s="2">
-        <v>3769.5732838589984</v>
+        <v>3189.9814471243044</v>
       </c>
       <c r="F2" s="2">
-        <v>225.53730158730156</v>
+        <v>226.99708994708996</v>
       </c>
       <c r="G2" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="H2" s="2">
-        <v>101.32835288704852</v>
+        <v>97.284467120181418</v>
       </c>
       <c r="I2" s="2">
-        <v>138.82608695652175</v>
+        <v>133.28571428571428</v>
       </c>
       <c r="J2" s="2">
-        <v>210.21</v>
+        <v>107.80000000000001</v>
       </c>
       <c r="K2" s="2">
-        <v>78</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1009,28 +1004,28 @@
         <v>3100</v>
       </c>
       <c r="D3" s="2">
-        <v>11387</v>
+        <v>9723</v>
       </c>
       <c r="E3" s="2">
-        <v>3673.2258064516127</v>
+        <v>3136.4516129032259</v>
       </c>
       <c r="F3" s="2">
-        <v>277.17896174863387</v>
+        <v>278.85883424408013</v>
       </c>
       <c r="G3" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="H3" s="2">
-        <v>124.52967846677754</v>
+        <v>119.51092896174863</v>
       </c>
       <c r="I3" s="2">
-        <v>148.2608695652174</v>
+        <v>142.28571428571428</v>
       </c>
       <c r="J3" s="2">
-        <v>155</v>
+        <v>85.25</v>
       </c>
       <c r="K3" s="2">
-        <v>50</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1044,28 +1039,28 @@
         <v>2800</v>
       </c>
       <c r="D4" s="2">
-        <v>10459</v>
+        <v>8864</v>
       </c>
       <c r="E4" s="2">
-        <v>3735.3571428571427</v>
+        <v>3165.7142857142858</v>
       </c>
       <c r="F4" s="2">
-        <v>304.83207070707073</v>
+        <v>311.23274410774411</v>
       </c>
       <c r="G4" s="2">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="H4" s="2">
-        <v>136.95353901332163</v>
+        <v>133.38546176046177</v>
       </c>
       <c r="I4" s="2">
-        <v>171.17391304347825</v>
+        <v>166.71428571428572</v>
       </c>
       <c r="J4" s="2">
-        <v>139.85999999999999</v>
+        <v>75.600000000000009</v>
       </c>
       <c r="K4" s="2">
-        <v>49.95</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1079,28 +1074,28 @@
         <v>6150</v>
       </c>
       <c r="D5" s="2">
-        <v>22184</v>
+        <v>19093</v>
       </c>
       <c r="E5" s="2">
-        <v>3607.1544715447153</v>
+        <v>3104.5528455284552</v>
       </c>
       <c r="F5" s="2">
-        <v>408.93424036281175</v>
+        <v>411.81405895691614</v>
       </c>
       <c r="G5" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="H5" s="2">
-        <v>183.72407900358209</v>
+        <v>176.49173955296408</v>
       </c>
       <c r="I5" s="2">
-        <v>127.59420289855072</v>
+        <v>122.57142857142857</v>
       </c>
       <c r="J5" s="2">
-        <v>219.678</v>
+        <v>132.04050000000001</v>
       </c>
       <c r="K5" s="2">
-        <v>35.72</v>
+        <v>21.47</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1114,28 +1109,28 @@
         <v>6430</v>
       </c>
       <c r="D6" s="2">
-        <v>23189</v>
+        <v>20098</v>
       </c>
       <c r="E6" s="2">
-        <v>3606.3763608087093</v>
+        <v>3125.660964230171</v>
       </c>
       <c r="F6" s="2">
-        <v>448.49649406688235</v>
+        <v>447.00647249190939</v>
       </c>
       <c r="G6" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H6" s="2">
-        <v>201.49842487062833</v>
+        <v>191.57420249653259</v>
       </c>
       <c r="I6" s="2">
-        <v>135.231884057971</v>
+        <v>128.57142857142858</v>
       </c>
       <c r="J6" s="2">
-        <v>362.65199999999999</v>
+        <v>216.048</v>
       </c>
       <c r="K6" s="2">
-        <v>56.4</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1149,28 +1144,28 @@
         <v>6435</v>
       </c>
       <c r="D7" s="2">
-        <v>23421</v>
+        <v>20264</v>
       </c>
       <c r="E7" s="2">
-        <v>3639.6270396270397</v>
+        <v>3149.0287490287492</v>
       </c>
       <c r="F7" s="2">
-        <v>351.52368421052626</v>
+        <v>352.78362573099417</v>
       </c>
       <c r="G7" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H7" s="2">
-        <v>157.93093058733788</v>
+        <v>151.19298245614036</v>
       </c>
       <c r="I7" s="2">
-        <v>125.34782608695652</v>
+        <v>120</v>
       </c>
       <c r="J7" s="2">
-        <v>305.66250000000002</v>
+        <v>168.91874999999999</v>
       </c>
       <c r="K7" s="2">
-        <v>47.5</v>
+        <v>26.25</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1184,28 +1179,28 @@
         <v>5890</v>
       </c>
       <c r="D8" s="2">
-        <v>21789</v>
+        <v>18529</v>
       </c>
       <c r="E8" s="2">
-        <v>3699.320882852292</v>
+        <v>3145.8404074702885</v>
       </c>
       <c r="F8" s="2">
-        <v>391.67676767676772</v>
+        <v>395.75673400673395</v>
       </c>
       <c r="G8" s="2">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="H8" s="2">
-        <v>175.97072170985214</v>
+        <v>169.61002886002882</v>
       </c>
       <c r="I8" s="2">
-        <v>129.39130434782609</v>
+        <v>124.71428571428571</v>
       </c>
       <c r="J8" s="2">
-        <v>250.61950000000002</v>
+        <v>155.79050000000001</v>
       </c>
       <c r="K8" s="2">
-        <v>42.55</v>
+        <v>26.450000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1219,28 +1214,28 @@
         <v>4980</v>
       </c>
       <c r="D9" s="2">
-        <v>19789</v>
+        <v>16199</v>
       </c>
       <c r="E9" s="2">
-        <v>3973.6947791164657</v>
+        <v>3252.8112449799196</v>
       </c>
       <c r="F9" s="2">
-        <v>334.61798679867985</v>
+        <v>338.06765676567653</v>
       </c>
       <c r="G9" s="2">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="H9" s="2">
-        <v>150.33561725737792</v>
+        <v>144.88613861386136</v>
       </c>
       <c r="I9" s="2">
-        <v>130.7391304347826</v>
+        <v>126</v>
       </c>
       <c r="J9" s="2">
-        <v>313.74</v>
+        <v>174.3</v>
       </c>
       <c r="K9" s="2">
-        <v>63</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1254,28 +1249,28 @@
         <v>7020</v>
       </c>
       <c r="D10" s="2">
-        <v>25126</v>
+        <v>21526</v>
       </c>
       <c r="E10" s="2">
-        <v>3579.202279202279</v>
+        <v>3066.3817663817663</v>
       </c>
       <c r="F10" s="2">
-        <v>676.8</v>
+        <v>682.44</v>
       </c>
       <c r="G10" s="2">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="H10" s="2">
-        <v>304.0695652173913</v>
+        <v>292.47428571428571</v>
       </c>
       <c r="I10" s="2">
-        <v>161.7391304347826</v>
+        <v>155.57142857142858</v>
       </c>
       <c r="J10" s="2">
-        <v>407.16</v>
+        <v>234.11700000000002</v>
       </c>
       <c r="K10" s="2">
-        <v>58</v>
+        <v>33.35</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1289,28 +1284,28 @@
         <v>5320</v>
       </c>
       <c r="D11" s="2">
-        <v>20485</v>
+        <v>16821</v>
       </c>
       <c r="E11" s="2">
-        <v>3850.5639097744361</v>
+        <v>3161.8421052631579</v>
       </c>
       <c r="F11" s="2">
-        <v>330.08765432098767</v>
+        <v>332.60740740740744</v>
       </c>
       <c r="G11" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="H11" s="2">
-        <v>148.30025049203795</v>
+        <v>142.54603174603176</v>
       </c>
       <c r="I11" s="2">
-        <v>117.71014492753623</v>
+        <v>113.14285714285714</v>
       </c>
       <c r="J11" s="2">
-        <v>283.024</v>
+        <v>171.30400000000003</v>
       </c>
       <c r="K11" s="2">
-        <v>53.20000000000001</v>
+        <v>32.20000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1324,28 +1319,28 @@
         <v>3570</v>
       </c>
       <c r="D12" s="2">
-        <v>18636</v>
+        <v>15123</v>
       </c>
       <c r="E12" s="2">
-        <v>5220.1680672268903</v>
+        <v>4236.134453781513</v>
       </c>
       <c r="F12" s="2">
-        <v>220.22740873728304</v>
+        <v>223.75104727707961</v>
       </c>
       <c r="G12" s="2">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="H12" s="2">
-        <v>98.942748852982234</v>
+        <v>95.893305975891266</v>
       </c>
       <c r="I12" s="2">
-        <v>112.31884057971014</v>
+        <v>108.85714285714286</v>
       </c>
       <c r="J12" s="2">
-        <v>167.184</v>
+        <v>83.591999999999999</v>
       </c>
       <c r="K12" s="2">
-        <v>43.199999999999996</v>
+        <v>21.599999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1359,28 +1354,28 @@
         <v>7356</v>
       </c>
       <c r="D13" s="2">
-        <v>26998</v>
+        <v>22569</v>
       </c>
       <c r="E13" s="2">
-        <v>3670.2011963023383</v>
+        <v>3068.1076672104405</v>
       </c>
       <c r="F13" s="2">
-        <v>461.00483425414365</v>
+        <v>509.31975138121544</v>
       </c>
       <c r="G13" s="2">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="H13" s="2">
-        <v>207.11811394026745</v>
+        <v>218.27989344909233</v>
       </c>
       <c r="I13" s="2">
-        <v>102.8840579710145</v>
+        <v>98</v>
       </c>
       <c r="J13" s="2">
-        <v>293.50439999999998</v>
+        <v>169.92359999999999</v>
       </c>
       <c r="K13" s="2">
-        <v>39.9</v>
+        <v>23.1</v>
       </c>
     </row>
   </sheetData>
@@ -1444,28 +1439,28 @@
         <v>2695</v>
       </c>
       <c r="D2" s="2">
-        <v>10850</v>
+        <v>10159</v>
       </c>
       <c r="E2" s="2">
-        <v>4025.9740259740261</v>
+        <v>3769.5732838589984</v>
       </c>
       <c r="F2" s="2">
-        <v>219.69814814814814</v>
+        <v>225.53730158730156</v>
       </c>
       <c r="G2" s="2">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="H2" s="2">
-        <v>103.38736383442266</v>
+        <v>101.32835288704852</v>
       </c>
       <c r="I2" s="2">
-        <v>141.64705882352942</v>
+        <v>138.82608695652175</v>
       </c>
       <c r="J2" s="2">
-        <v>203.74199999999999</v>
+        <v>210.21</v>
       </c>
       <c r="K2" s="2">
-        <v>75.599999999999994</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1479,28 +1474,28 @@
         <v>3100</v>
       </c>
       <c r="D3" s="2">
-        <v>11882</v>
+        <v>11387</v>
       </c>
       <c r="E3" s="2">
-        <v>3832.9032258064517</v>
+        <v>3673.2258064516127</v>
       </c>
       <c r="F3" s="2">
-        <v>276.33902550091074</v>
+        <v>277.17896174863387</v>
       </c>
       <c r="G3" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H3" s="2">
-        <v>130.04189435336977</v>
+        <v>124.52967846677754</v>
       </c>
       <c r="I3" s="2">
-        <v>154.8235294117647</v>
+        <v>148.2608695652174</v>
       </c>
       <c r="J3" s="2">
-        <v>127.875</v>
+        <v>155</v>
       </c>
       <c r="K3" s="2">
-        <v>41.25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1514,28 +1509,28 @@
         <v>2800</v>
       </c>
       <c r="D4" s="2">
-        <v>10985</v>
+        <v>10459</v>
       </c>
       <c r="E4" s="2">
-        <v>3923.2142857142858</v>
+        <v>3735.3571428571427</v>
       </c>
       <c r="F4" s="2">
-        <v>303.23190235690237</v>
+        <v>304.83207070707073</v>
       </c>
       <c r="G4" s="2">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="H4" s="2">
-        <v>142.69736581501289</v>
+        <v>136.95353901332163</v>
       </c>
       <c r="I4" s="2">
-        <v>178.35294117647058</v>
+        <v>171.17391304347825</v>
       </c>
       <c r="J4" s="2">
-        <v>136.07999999999998</v>
+        <v>139.85999999999999</v>
       </c>
       <c r="K4" s="2">
-        <v>48.6</v>
+        <v>49.95</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1549,10 +1544,10 @@
         <v>6150</v>
       </c>
       <c r="D5" s="2">
-        <v>23646</v>
+        <v>22184</v>
       </c>
       <c r="E5" s="2">
-        <v>3844.8780487804879</v>
+        <v>3607.1544715447153</v>
       </c>
       <c r="F5" s="2">
         <v>408.93424036281175</v>
@@ -1561,16 +1556,16 @@
         <v>284</v>
       </c>
       <c r="H5" s="2">
-        <v>192.43964252367613</v>
+        <v>183.72407900358209</v>
       </c>
       <c r="I5" s="2">
-        <v>133.64705882352942</v>
+        <v>127.59420289855072</v>
       </c>
       <c r="J5" s="2">
-        <v>212.667</v>
+        <v>219.678</v>
       </c>
       <c r="K5" s="2">
-        <v>34.58</v>
+        <v>35.72</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1584,10 +1579,10 @@
         <v>6430</v>
       </c>
       <c r="D6" s="2">
-        <v>24623</v>
+        <v>23189</v>
       </c>
       <c r="E6" s="2">
-        <v>3829.3934681181959</v>
+        <v>3606.3763608087093</v>
       </c>
       <c r="F6" s="2">
         <v>448.49649406688235</v>
@@ -1596,16 +1591,16 @@
         <v>301</v>
       </c>
       <c r="H6" s="2">
-        <v>211.05717367853288</v>
+        <v>201.49842487062833</v>
       </c>
       <c r="I6" s="2">
-        <v>141.64705882352942</v>
+        <v>135.231884057971</v>
       </c>
       <c r="J6" s="2">
-        <v>343.36199999999997</v>
+        <v>362.65199999999999</v>
       </c>
       <c r="K6" s="2">
-        <v>53.4</v>
+        <v>56.4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1619,28 +1614,28 @@
         <v>6435</v>
       </c>
       <c r="D7" s="2">
-        <v>24856</v>
+        <v>23421</v>
       </c>
       <c r="E7" s="2">
-        <v>3862.6262626262628</v>
+        <v>3639.6270396270397</v>
       </c>
       <c r="F7" s="2">
-        <v>349.00380116959059</v>
+        <v>351.52368421052626</v>
       </c>
       <c r="G7" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="H7" s="2">
-        <v>164.23708290333676</v>
+        <v>157.93093058733788</v>
       </c>
       <c r="I7" s="2">
-        <v>130.35294117647058</v>
+        <v>125.34782608695652</v>
       </c>
       <c r="J7" s="2">
-        <v>292.79250000000002</v>
+        <v>305.66250000000002</v>
       </c>
       <c r="K7" s="2">
-        <v>45.5</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1654,10 +1649,10 @@
         <v>5890</v>
       </c>
       <c r="D8" s="2">
-        <v>23589</v>
+        <v>21789</v>
       </c>
       <c r="E8" s="2">
-        <v>4004.9235993208827</v>
+        <v>3699.320882852292</v>
       </c>
       <c r="F8" s="2">
         <v>391.67676767676772</v>
@@ -1666,16 +1661,16 @@
         <v>288</v>
       </c>
       <c r="H8" s="2">
-        <v>184.31847890671423</v>
+        <v>175.97072170985214</v>
       </c>
       <c r="I8" s="2">
-        <v>135.52941176470588</v>
+        <v>129.39130434782609</v>
       </c>
       <c r="J8" s="2">
-        <v>246.55539999999999</v>
+        <v>250.61950000000002</v>
       </c>
       <c r="K8" s="2">
-        <v>41.86</v>
+        <v>42.55</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1689,28 +1684,28 @@
         <v>4980</v>
       </c>
       <c r="D9" s="2">
-        <v>21498</v>
+        <v>19789</v>
       </c>
       <c r="E9" s="2">
-        <v>4316.8674698795185</v>
+        <v>3973.6947791164657</v>
       </c>
       <c r="F9" s="2">
-        <v>332.31820682068201</v>
+        <v>334.61798679867985</v>
       </c>
       <c r="G9" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="H9" s="2">
-        <v>156.38503850385035</v>
+        <v>150.33561725737792</v>
       </c>
       <c r="I9" s="2">
-        <v>136</v>
+        <v>130.7391304347826</v>
       </c>
       <c r="J9" s="2">
-        <v>329.42700000000002</v>
+        <v>313.74</v>
       </c>
       <c r="K9" s="2">
-        <v>66.150000000000006</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1724,28 +1719,28 @@
         <v>7020</v>
       </c>
       <c r="D10" s="2">
-        <v>25925</v>
+        <v>25126</v>
       </c>
       <c r="E10" s="2">
-        <v>3693.0199430199432</v>
+        <v>3579.202279202279</v>
       </c>
       <c r="F10" s="2">
-        <v>682.44</v>
+        <v>676.8</v>
       </c>
       <c r="G10" s="2">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="H10" s="2">
-        <v>321.14823529411768</v>
+        <v>304.0695652173913</v>
       </c>
       <c r="I10" s="2">
-        <v>170.8235294117647</v>
+        <v>161.7391304347826</v>
       </c>
       <c r="J10" s="2">
-        <v>356.26499999999999</v>
+        <v>407.16</v>
       </c>
       <c r="K10" s="2">
-        <v>50.75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1759,28 +1754,28 @@
         <v>5320</v>
       </c>
       <c r="D11" s="2">
-        <v>21603</v>
+        <v>20485</v>
       </c>
       <c r="E11" s="2">
-        <v>4060.7142857142858</v>
+        <v>3850.5639097744361</v>
       </c>
       <c r="F11" s="2">
-        <v>327.5679012345679</v>
+        <v>330.08765432098767</v>
       </c>
       <c r="G11" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="H11" s="2">
-        <v>154.14960058097313</v>
+        <v>148.30025049203795</v>
       </c>
       <c r="I11" s="2">
-        <v>122.35294117647059</v>
+        <v>117.71014492753623</v>
       </c>
       <c r="J11" s="2">
-        <v>275.57600000000002</v>
+        <v>283.024</v>
       </c>
       <c r="K11" s="2">
-        <v>51.800000000000011</v>
+        <v>53.20000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1794,28 +1789,28 @@
         <v>3570</v>
       </c>
       <c r="D12" s="2">
-        <v>19256</v>
+        <v>18636</v>
       </c>
       <c r="E12" s="2">
-        <v>5393.8375350140059</v>
+        <v>5220.1680672268903</v>
       </c>
       <c r="F12" s="2">
-        <v>221.10831837223216</v>
+        <v>220.22740873728304</v>
       </c>
       <c r="G12" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H12" s="2">
-        <v>104.05097335163866</v>
+        <v>98.942748852982234</v>
       </c>
       <c r="I12" s="2">
-        <v>118.11764705882354</v>
+        <v>112.31884057971014</v>
       </c>
       <c r="J12" s="2">
-        <v>175.54319999999998</v>
+        <v>167.184</v>
       </c>
       <c r="K12" s="2">
-        <v>45.36</v>
+        <v>43.199999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1829,33 +1824,32 @@
         <v>7356</v>
       </c>
       <c r="D13" s="2">
-        <v>26832</v>
+        <v>26998</v>
       </c>
       <c r="E13" s="2">
-        <v>3647.6345840130507</v>
+        <v>3670.2011963023383</v>
       </c>
       <c r="F13" s="2">
-        <v>458.99171270718233</v>
+        <v>461.00483425414365</v>
       </c>
       <c r="G13" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H13" s="2">
-        <v>215.99610009749756</v>
+        <v>207.11811394026745</v>
       </c>
       <c r="I13" s="2">
-        <v>107.29411764705883</v>
+        <v>102.8840579710145</v>
       </c>
       <c r="J13" s="2">
-        <v>278.05680000000001</v>
+        <v>293.50439999999998</v>
       </c>
       <c r="K13" s="2">
-        <v>37.799999999999997</v>
+        <v>39.9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1864,7 +1858,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K13"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,28 +1909,28 @@
         <v>2695</v>
       </c>
       <c r="D2" s="2">
-        <v>9797</v>
+        <v>10850</v>
       </c>
       <c r="E2" s="2">
-        <v>3635.2504638218925</v>
+        <v>4025.9740259740261</v>
       </c>
       <c r="F2" s="2">
-        <v>220.42804232804232</v>
+        <v>219.69814814814814</v>
       </c>
       <c r="G2" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H2" s="2">
-        <v>99.032888582163935</v>
+        <v>103.38736383442266</v>
       </c>
       <c r="I2" s="2">
-        <v>135.68115942028984</v>
+        <v>141.64705882352942</v>
       </c>
       <c r="J2" s="2">
-        <v>188.64999999999998</v>
+        <v>203.74199999999999</v>
       </c>
       <c r="K2" s="2">
-        <v>70</v>
+        <v>75.599999999999994</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1950,28 +1944,28 @@
         <v>3100</v>
       </c>
       <c r="D3" s="2">
-        <v>10697</v>
+        <v>11882</v>
       </c>
       <c r="E3" s="2">
-        <v>3450.6451612903224</v>
+        <v>3832.9032258064517</v>
       </c>
       <c r="F3" s="2">
-        <v>374.61156648451731</v>
+        <v>276.33902550091074</v>
       </c>
       <c r="G3" s="2">
-        <v>446</v>
+        <v>329</v>
       </c>
       <c r="H3" s="2">
-        <v>168.30374726115997</v>
+        <v>130.04189435336977</v>
       </c>
       <c r="I3" s="2">
-        <v>200.37681159420291</v>
+        <v>154.8235294117647</v>
       </c>
       <c r="J3" s="2">
-        <v>124</v>
+        <v>127.875</v>
       </c>
       <c r="K3" s="2">
-        <v>40</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1985,22 +1979,22 @@
         <v>2800</v>
       </c>
       <c r="D4" s="2">
-        <v>10069</v>
+        <v>10985</v>
       </c>
       <c r="E4" s="2">
-        <v>3596.0714285714284</v>
+        <v>3923.2142857142858</v>
       </c>
       <c r="F4" s="2">
-        <v>304.83207070707073</v>
+        <v>303.23190235690237</v>
       </c>
       <c r="G4" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H4" s="2">
-        <v>136.95353901332163</v>
+        <v>142.69736581501289</v>
       </c>
       <c r="I4" s="2">
-        <v>171.17391304347825</v>
+        <v>178.35294117647058</v>
       </c>
       <c r="J4" s="2">
         <v>136.07999999999998</v>
@@ -2020,10 +2014,10 @@
         <v>6150</v>
       </c>
       <c r="D5" s="2">
-        <v>21938</v>
+        <v>23646</v>
       </c>
       <c r="E5" s="2">
-        <v>3567.1544715447153</v>
+        <v>3844.8780487804879</v>
       </c>
       <c r="F5" s="2">
         <v>408.93424036281175</v>
@@ -2032,16 +2026,16 @@
         <v>284</v>
       </c>
       <c r="H5" s="2">
-        <v>183.72407900358209</v>
+        <v>192.43964252367613</v>
       </c>
       <c r="I5" s="2">
-        <v>127.59420289855072</v>
+        <v>133.64705882352942</v>
       </c>
       <c r="J5" s="2">
-        <v>204.48749999999998</v>
+        <v>212.667</v>
       </c>
       <c r="K5" s="2">
-        <v>33.25</v>
+        <v>34.58</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2055,28 +2049,28 @@
         <v>6430</v>
       </c>
       <c r="D6" s="2">
-        <v>21903</v>
+        <v>24623</v>
       </c>
       <c r="E6" s="2">
-        <v>3406.3763608087093</v>
+        <v>3829.3934681181959</v>
       </c>
       <c r="F6" s="2">
-        <v>447.00647249190939</v>
+        <v>448.49649406688235</v>
       </c>
       <c r="G6" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H6" s="2">
-        <v>200.82899488766944</v>
+        <v>211.05717367853288</v>
       </c>
       <c r="I6" s="2">
-        <v>134.78260869565219</v>
+        <v>141.64705882352942</v>
       </c>
       <c r="J6" s="2">
-        <v>322.14300000000003</v>
+        <v>343.36199999999997</v>
       </c>
       <c r="K6" s="2">
-        <v>50.1</v>
+        <v>53.4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2090,28 +2084,28 @@
         <v>6435</v>
       </c>
       <c r="D7" s="2">
-        <v>22231</v>
+        <v>24856</v>
       </c>
       <c r="E7" s="2">
-        <v>3454.7008547008545</v>
+        <v>3862.6262626262628</v>
       </c>
       <c r="F7" s="2">
-        <v>347.74385964912284</v>
+        <v>349.00380116959059</v>
       </c>
       <c r="G7" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H7" s="2">
-        <v>156.23274853801172</v>
+        <v>164.23708290333676</v>
       </c>
       <c r="I7" s="2">
-        <v>124</v>
+        <v>130.35294117647058</v>
       </c>
       <c r="J7" s="2">
-        <v>281.53125</v>
+        <v>292.79250000000002</v>
       </c>
       <c r="K7" s="2">
-        <v>43.75</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2125,28 +2119,28 @@
         <v>5890</v>
       </c>
       <c r="D8" s="2">
-        <v>21498</v>
+        <v>23589</v>
       </c>
       <c r="E8" s="2">
-        <v>3649.9151103565364</v>
+        <v>4004.9235993208827</v>
       </c>
       <c r="F8" s="2">
-        <v>388.95679012345681</v>
+        <v>391.67676767676772</v>
       </c>
       <c r="G8" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="H8" s="2">
-        <v>174.74870280908928</v>
+        <v>184.31847890671423</v>
       </c>
       <c r="I8" s="2">
-        <v>128.49275362318841</v>
+        <v>135.52941176470588</v>
       </c>
       <c r="J8" s="2">
-        <v>237.07249999999999</v>
+        <v>246.55539999999999</v>
       </c>
       <c r="K8" s="2">
-        <v>40.25</v>
+        <v>41.86</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2160,28 +2154,28 @@
         <v>4980</v>
       </c>
       <c r="D9" s="2">
-        <v>18898</v>
+        <v>21498</v>
       </c>
       <c r="E9" s="2">
-        <v>3794.7791164658634</v>
+        <v>4316.8674698795185</v>
       </c>
       <c r="F9" s="2">
-        <v>333.46809680968096</v>
+        <v>332.31820682068201</v>
       </c>
       <c r="G9" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H9" s="2">
-        <v>149.8190000159436</v>
+        <v>156.38503850385035</v>
       </c>
       <c r="I9" s="2">
-        <v>130.28985507246378</v>
+        <v>136</v>
       </c>
       <c r="J9" s="2">
-        <v>311.99700000000001</v>
+        <v>329.42700000000002</v>
       </c>
       <c r="K9" s="2">
-        <v>62.65</v>
+        <v>66.150000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2195,28 +2189,28 @@
         <v>7020</v>
       </c>
       <c r="D10" s="2">
-        <v>23210</v>
+        <v>25925</v>
       </c>
       <c r="E10" s="2">
-        <v>3306.2678062678065</v>
+        <v>3693.0199430199432</v>
       </c>
       <c r="F10" s="2">
-        <v>678.68</v>
+        <v>682.44</v>
       </c>
       <c r="G10" s="2">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="H10" s="2">
-        <v>304.91420289855068</v>
+        <v>321.14823529411768</v>
       </c>
       <c r="I10" s="2">
-        <v>162.18840579710144</v>
+        <v>170.8235294117647</v>
       </c>
       <c r="J10" s="2">
-        <v>335.90699999999998</v>
+        <v>356.26499999999999</v>
       </c>
       <c r="K10" s="2">
-        <v>47.85</v>
+        <v>50.75</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2230,28 +2224,28 @@
         <v>5320</v>
       </c>
       <c r="D11" s="2">
-        <v>19503</v>
+        <v>21603</v>
       </c>
       <c r="E11" s="2">
-        <v>3665.9774436090224</v>
+        <v>4060.7142857142858</v>
       </c>
       <c r="F11" s="2">
-        <v>325.04814814814813</v>
+        <v>327.5679012345679</v>
       </c>
       <c r="G11" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="H11" s="2">
-        <v>146.03612453032744</v>
+        <v>154.14960058097313</v>
       </c>
       <c r="I11" s="2">
-        <v>115.91304347826087</v>
+        <v>122.35294117647059</v>
       </c>
       <c r="J11" s="2">
-        <v>260.68</v>
+        <v>275.57600000000002</v>
       </c>
       <c r="K11" s="2">
-        <v>49.000000000000007</v>
+        <v>51.800000000000011</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2265,28 +2259,28 @@
         <v>3570</v>
       </c>
       <c r="D12" s="2">
-        <v>17396</v>
+        <v>19256</v>
       </c>
       <c r="E12" s="2">
-        <v>4872.8291316526611</v>
+        <v>5393.8375350140059</v>
       </c>
       <c r="F12" s="2">
-        <v>222.87013764213046</v>
+        <v>221.10831837223216</v>
       </c>
       <c r="G12" s="2">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H12" s="2">
-        <v>100.13006183921803</v>
+        <v>104.05097335163866</v>
       </c>
       <c r="I12" s="2">
-        <v>113.66666666666667</v>
+        <v>118.11764705882354</v>
       </c>
       <c r="J12" s="2">
-        <v>166.25519999999997</v>
+        <v>175.54319999999998</v>
       </c>
       <c r="K12" s="2">
-        <v>42.96</v>
+        <v>45.36</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2300,28 +2294,28 @@
         <v>7356</v>
       </c>
       <c r="D13" s="2">
-        <v>23985</v>
+        <v>26832</v>
       </c>
       <c r="E13" s="2">
-        <v>3260.6035889070145</v>
+        <v>3647.6345840130507</v>
       </c>
       <c r="F13" s="2">
-        <v>467.04419889502765</v>
+        <v>458.99171270718233</v>
       </c>
       <c r="G13" s="2">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H13" s="2">
-        <v>209.8314516774762</v>
+        <v>215.99610009749756</v>
       </c>
       <c r="I13" s="2">
-        <v>104.23188405797102</v>
+        <v>107.29411764705883</v>
       </c>
       <c r="J13" s="2">
-        <v>247.16159999999999</v>
+        <v>278.05680000000001</v>
       </c>
       <c r="K13" s="2">
-        <v>33.6</v>
+        <v>37.799999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2331,6 +2325,482 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2695</v>
+      </c>
+      <c r="D2" s="2">
+        <v>7598</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2819.294990723562</v>
+      </c>
+      <c r="F2" s="2">
+        <v>222.61772486772483</v>
+      </c>
+      <c r="G2" s="2">
+        <v>305</v>
+      </c>
+      <c r="H2" s="2">
+        <v>95.407596371882065</v>
+      </c>
+      <c r="I2" s="2">
+        <v>130.71428571428572</v>
+      </c>
+      <c r="J2" s="2">
+        <v>134.75</v>
+      </c>
+      <c r="K2" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3100</v>
+      </c>
+      <c r="D3" s="2">
+        <v>8496</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2740.6451612903224</v>
+      </c>
+      <c r="F3" s="2">
+        <v>364.53233151183974</v>
+      </c>
+      <c r="G3" s="2">
+        <v>434</v>
+      </c>
+      <c r="H3" s="2">
+        <v>156.22814207650276</v>
+      </c>
+      <c r="I3" s="2">
+        <v>151</v>
+      </c>
+      <c r="J3" s="2">
+        <v>116.25</v>
+      </c>
+      <c r="K3" s="2">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2800</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7885</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2816.0714285714284</v>
+      </c>
+      <c r="F4" s="2">
+        <v>306.43223905723903</v>
+      </c>
+      <c r="G4" s="2">
+        <v>383</v>
+      </c>
+      <c r="H4" s="2">
+        <v>131.32810245310245</v>
+      </c>
+      <c r="I4" s="2">
+        <v>164.14285714285714</v>
+      </c>
+      <c r="J4" s="2">
+        <v>113.39999999999999</v>
+      </c>
+      <c r="K4" s="2">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>69</v>
+      </c>
+      <c r="C5" s="2">
+        <v>6150</v>
+      </c>
+      <c r="D5" s="2">
+        <v>17696</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2877.3983739837399</v>
+      </c>
+      <c r="F5" s="2">
+        <v>407.4943310657597</v>
+      </c>
+      <c r="G5" s="2">
+        <v>283</v>
+      </c>
+      <c r="H5" s="2">
+        <v>174.64042759961129</v>
+      </c>
+      <c r="I5" s="2">
+        <v>121.28571428571429</v>
+      </c>
+      <c r="J5" s="2">
+        <v>169.43249999999998</v>
+      </c>
+      <c r="K5" s="2">
+        <v>27.549999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>71</v>
+      </c>
+      <c r="C6" s="2">
+        <v>6430</v>
+      </c>
+      <c r="D6" s="2">
+        <v>18769</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2918.9735614307933</v>
+      </c>
+      <c r="F6" s="2">
+        <v>449.98651564185542</v>
+      </c>
+      <c r="G6" s="2">
+        <v>302</v>
+      </c>
+      <c r="H6" s="2">
+        <v>192.85136384650946</v>
+      </c>
+      <c r="I6" s="2">
+        <v>129.42857142857142</v>
+      </c>
+      <c r="J6" s="2">
+        <v>279.70499999999998</v>
+      </c>
+      <c r="K6" s="2">
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>70</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6435</v>
+      </c>
+      <c r="D7" s="2">
+        <v>19002</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2952.9137529137529</v>
+      </c>
+      <c r="F7" s="2">
+        <v>341.44415204678364</v>
+      </c>
+      <c r="G7" s="2">
+        <v>271</v>
+      </c>
+      <c r="H7" s="2">
+        <v>146.33320802005014</v>
+      </c>
+      <c r="I7" s="2">
+        <v>116.14285714285714</v>
+      </c>
+      <c r="J7" s="2">
+        <v>225.22500000000002</v>
+      </c>
+      <c r="K7" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>55</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5890</v>
+      </c>
+      <c r="D8" s="2">
+        <v>17059</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2896.2648556876061</v>
+      </c>
+      <c r="F8" s="2">
+        <v>390.31677890011224</v>
+      </c>
+      <c r="G8" s="2">
+        <v>287</v>
+      </c>
+      <c r="H8" s="2">
+        <v>167.27861952861952</v>
+      </c>
+      <c r="I8" s="2">
+        <v>123</v>
+      </c>
+      <c r="J8" s="2">
+        <v>189.65800000000002</v>
+      </c>
+      <c r="K8" s="2">
+        <v>32.200000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>48</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4980</v>
+      </c>
+      <c r="D9" s="2">
+        <v>15074</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3026.9076305220883</v>
+      </c>
+      <c r="F9" s="2">
+        <v>334.61798679867985</v>
+      </c>
+      <c r="G9" s="2">
+        <v>291</v>
+      </c>
+      <c r="H9" s="2">
+        <v>143.40770862800565</v>
+      </c>
+      <c r="I9" s="2">
+        <v>124.71428571428571</v>
+      </c>
+      <c r="J9" s="2">
+        <v>259.70699999999999</v>
+      </c>
+      <c r="K9" s="2">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>90</v>
+      </c>
+      <c r="C10" s="2">
+        <v>7020</v>
+      </c>
+      <c r="D10" s="2">
+        <v>20629</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2938.6039886039885</v>
+      </c>
+      <c r="F10" s="2">
+        <v>678.68</v>
+      </c>
+      <c r="G10" s="2">
+        <v>361</v>
+      </c>
+      <c r="H10" s="2">
+        <v>290.86285714285714</v>
+      </c>
+      <c r="I10" s="2">
+        <v>154.71428571428572</v>
+      </c>
+      <c r="J10" s="2">
+        <v>285.012</v>
+      </c>
+      <c r="K10" s="2">
+        <v>40.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>60</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5320</v>
+      </c>
+      <c r="D11" s="2">
+        <v>15249</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2866.3533834586465</v>
+      </c>
+      <c r="F11" s="2">
+        <v>327.5679012345679</v>
+      </c>
+      <c r="G11" s="2">
+        <v>260</v>
+      </c>
+      <c r="H11" s="2">
+        <v>140.38624338624336</v>
+      </c>
+      <c r="I11" s="2">
+        <v>111.42857142857143</v>
+      </c>
+      <c r="J11" s="2">
+        <v>201.39392000000001</v>
+      </c>
+      <c r="K11" s="2">
+        <v>37.856000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3570</v>
+      </c>
+      <c r="D12" s="2">
+        <v>15514</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4345.6582633053222</v>
+      </c>
+      <c r="F12" s="2">
+        <v>219.34649910233392</v>
+      </c>
+      <c r="G12" s="2">
+        <v>249</v>
+      </c>
+      <c r="H12" s="2">
+        <v>94.005642472428832</v>
+      </c>
+      <c r="I12" s="2">
+        <v>106.71428571428571</v>
+      </c>
+      <c r="J12" s="2">
+        <v>130.03200000000001</v>
+      </c>
+      <c r="K12" s="2">
+        <v>33.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2">
+        <v>98</v>
+      </c>
+      <c r="C13" s="2">
+        <v>7356</v>
+      </c>
+      <c r="D13" s="2">
+        <v>21231</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2886.2153344208809</v>
+      </c>
+      <c r="F13" s="2">
+        <v>463.01795580110496</v>
+      </c>
+      <c r="G13" s="2">
+        <v>230</v>
+      </c>
+      <c r="H13" s="2">
+        <v>198.43626677190213</v>
+      </c>
+      <c r="I13" s="2">
+        <v>98.571428571428569</v>
+      </c>
+      <c r="J13" s="2">
+        <v>213.17688000000001</v>
+      </c>
+      <c r="K13" s="2">
+        <v>28.980000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -2813,7 +3283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
@@ -3290,476 +3760,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2695</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2587</v>
-      </c>
-      <c r="E2" s="2">
-        <v>711.64284985199549</v>
-      </c>
-      <c r="F2" s="2">
-        <v>244.51455026455028</v>
-      </c>
-      <c r="G2" s="2">
-        <v>335</v>
-      </c>
-      <c r="H2" s="2">
-        <v>64.997538677918428</v>
-      </c>
-      <c r="I2" s="2">
-        <v>89.050632911392398</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>40</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3100</v>
-      </c>
-      <c r="D3" s="2">
-        <v>3529</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1022.7073011124614</v>
-      </c>
-      <c r="F3" s="2">
-        <v>305.73679417122037</v>
-      </c>
-      <c r="G3" s="2">
-        <v>364</v>
-      </c>
-      <c r="H3" s="2">
-        <v>81.271806045514282</v>
-      </c>
-      <c r="I3" s="2">
-        <v>96.759493670886073</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>38</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2800</v>
-      </c>
-      <c r="D4" s="2">
-        <v>2810</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1003.5714285714286</v>
-      </c>
-      <c r="F4" s="2">
-        <v>340.03577441077437</v>
-      </c>
-      <c r="G4" s="2">
-        <v>425</v>
-      </c>
-      <c r="H4" s="2">
-        <v>90.389256488940021</v>
-      </c>
-      <c r="I4" s="2">
-        <v>112.9746835443038</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>69</v>
-      </c>
-      <c r="C5" s="2">
-        <v>6150</v>
-      </c>
-      <c r="D5" s="2">
-        <v>7287</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1184.8780487804879</v>
-      </c>
-      <c r="F5" s="2">
-        <v>455.01133786848072</v>
-      </c>
-      <c r="G5" s="2">
-        <v>316</v>
-      </c>
-      <c r="H5" s="2">
-        <v>120.95238095238095</v>
-      </c>
-      <c r="I5" s="2">
-        <v>84</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>71</v>
-      </c>
-      <c r="C6" s="2">
-        <v>6430</v>
-      </c>
-      <c r="D6" s="2">
-        <v>7801</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1213.2192846034216</v>
-      </c>
-      <c r="F6" s="2">
-        <v>496.17718446601941</v>
-      </c>
-      <c r="G6" s="2">
-        <v>333</v>
-      </c>
-      <c r="H6" s="2">
-        <v>131.89520093400515</v>
-      </c>
-      <c r="I6" s="2">
-        <v>88.518987341772146</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>70</v>
-      </c>
-      <c r="C7" s="2">
-        <v>6435</v>
-      </c>
-      <c r="D7" s="2">
-        <v>8264</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1284.2268842268843</v>
-      </c>
-      <c r="F7" s="2">
-        <v>393.10175438596491</v>
-      </c>
-      <c r="G7" s="2">
-        <v>312</v>
-      </c>
-      <c r="H7" s="2">
-        <v>104.49540306462359</v>
-      </c>
-      <c r="I7" s="2">
-        <v>82.936708860759495</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
-        <v>55</v>
-      </c>
-      <c r="C8" s="2">
-        <v>5890</v>
-      </c>
-      <c r="D8" s="2">
-        <v>6921</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1175.0424448217318</v>
-      </c>
-      <c r="F8" s="2">
-        <v>436.55639730639734</v>
-      </c>
-      <c r="G8" s="2">
-        <v>321</v>
-      </c>
-      <c r="H8" s="2">
-        <v>116.04663725866259</v>
-      </c>
-      <c r="I8" s="2">
-        <v>85.329113924050631</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>48</v>
-      </c>
-      <c r="C9" s="2">
-        <v>4980</v>
-      </c>
-      <c r="D9" s="2">
-        <v>4028</v>
-      </c>
-      <c r="E9" s="2">
-        <v>808.83534136546189</v>
-      </c>
-      <c r="F9" s="2">
-        <v>378.31380638063803</v>
-      </c>
-      <c r="G9" s="2">
-        <v>329</v>
-      </c>
-      <c r="H9" s="2">
-        <v>100.56442954422023</v>
-      </c>
-      <c r="I9" s="2">
-        <v>87.455696202531641</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2">
-        <v>90</v>
-      </c>
-      <c r="C10" s="2">
-        <v>7020</v>
-      </c>
-      <c r="D10" s="2">
-        <v>6123</v>
-      </c>
-      <c r="E10" s="2">
-        <v>872.22222222222217</v>
-      </c>
-      <c r="F10" s="2">
-        <v>746.36</v>
-      </c>
-      <c r="G10" s="2">
-        <v>397</v>
-      </c>
-      <c r="H10" s="2">
-        <v>198.39949367088607</v>
-      </c>
-      <c r="I10" s="2">
-        <v>105.53164556962025</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
-        <v>60</v>
-      </c>
-      <c r="C11" s="2">
-        <v>5320</v>
-      </c>
-      <c r="D11" s="2">
-        <v>5365</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1008.4586466165414</v>
-      </c>
-      <c r="F11" s="2">
-        <v>364.10432098765438</v>
-      </c>
-      <c r="G11" s="2">
-        <v>289</v>
-      </c>
-      <c r="H11" s="2">
-        <v>96.787224566338494</v>
-      </c>
-      <c r="I11" s="2">
-        <v>76.822784810126578</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2">
-        <v>45</v>
-      </c>
-      <c r="C12" s="2">
-        <v>3570</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2889</v>
-      </c>
-      <c r="E12" s="2">
-        <v>809.24369747899163</v>
-      </c>
-      <c r="F12" s="2">
-        <v>310.08019150209458</v>
-      </c>
-      <c r="G12" s="2">
-        <v>352</v>
-      </c>
-      <c r="H12" s="2">
-        <v>82.426380019544126</v>
-      </c>
-      <c r="I12" s="2">
-        <v>93.569620253164558</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="2">
-        <v>98</v>
-      </c>
-      <c r="C13" s="2">
-        <v>7356</v>
-      </c>
-      <c r="D13" s="2">
-        <v>7896</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1073.4094616639477</v>
-      </c>
-      <c r="F13" s="2">
-        <v>513.34599447513801</v>
-      </c>
-      <c r="G13" s="2">
-        <v>255</v>
-      </c>
-      <c r="H13" s="2">
-        <v>136.45906182250505</v>
-      </c>
-      <c r="I13" s="2">
-        <v>67.784810126582272</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
@@ -3816,22 +3816,22 @@
         <v>2695</v>
       </c>
       <c r="D2" s="2">
-        <v>3298</v>
+        <v>2587</v>
       </c>
       <c r="E2" s="2">
-        <v>1169.7959989470914</v>
+        <v>711.64284985199549</v>
       </c>
       <c r="F2" s="2">
-        <v>245.9743386243386</v>
+        <v>244.51455026455028</v>
       </c>
       <c r="G2" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="H2" s="2">
-        <v>74.861755233494364</v>
+        <v>64.997538677918428</v>
       </c>
       <c r="I2" s="2">
-        <v>102.56521739130434</v>
+        <v>89.050632911392398</v>
       </c>
       <c r="J2" s="2">
         <v>0</v>
@@ -3851,10 +3851,10 @@
         <v>3100</v>
       </c>
       <c r="D3" s="2">
-        <v>4084</v>
+        <v>3529</v>
       </c>
       <c r="E3" s="2">
-        <v>1317.4193548387098</v>
+        <v>1022.7073011124614</v>
       </c>
       <c r="F3" s="2">
         <v>305.73679417122037</v>
@@ -3863,10 +3863,10 @@
         <v>364</v>
       </c>
       <c r="H3" s="2">
-        <v>93.050328660806201</v>
+        <v>81.271806045514282</v>
       </c>
       <c r="I3" s="2">
-        <v>110.78260869565217</v>
+        <v>96.759493670886073</v>
       </c>
       <c r="J3" s="2">
         <v>0</v>
@@ -3886,22 +3886,22 @@
         <v>2800</v>
       </c>
       <c r="D4" s="2">
-        <v>3385</v>
+        <v>2810</v>
       </c>
       <c r="E4" s="2">
-        <v>1208.9285714285713</v>
+        <v>1003.5714285714286</v>
       </c>
       <c r="F4" s="2">
-        <v>337.63552188552188</v>
+        <v>340.03577441077437</v>
       </c>
       <c r="G4" s="2">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="H4" s="2">
-        <v>102.75863709559361</v>
+        <v>90.389256488940021</v>
       </c>
       <c r="I4" s="2">
-        <v>128.43478260869566</v>
+        <v>112.9746835443038</v>
       </c>
       <c r="J4" s="2">
         <v>0</v>
@@ -3921,22 +3921,22 @@
         <v>6150</v>
       </c>
       <c r="D5" s="2">
-        <v>8628</v>
+        <v>7287</v>
       </c>
       <c r="E5" s="2">
-        <v>1402.9268292682927</v>
+        <v>1184.8780487804879</v>
       </c>
       <c r="F5" s="2">
-        <v>456.45124716553283</v>
+        <v>455.01133786848072</v>
       </c>
       <c r="G5" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H5" s="2">
-        <v>138.91994478951</v>
+        <v>120.95238095238095</v>
       </c>
       <c r="I5" s="2">
-        <v>96.478260869565219</v>
+        <v>84</v>
       </c>
       <c r="J5" s="2">
         <v>0</v>
@@ -3956,22 +3956,22 @@
         <v>6430</v>
       </c>
       <c r="D6" s="2">
-        <v>9602</v>
+        <v>7801</v>
       </c>
       <c r="E6" s="2">
-        <v>1493.3125972006221</v>
+        <v>1213.2192846034216</v>
       </c>
       <c r="F6" s="2">
-        <v>497.66720604099248</v>
+        <v>496.17718446601941</v>
       </c>
       <c r="G6" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H6" s="2">
-        <v>151.46393227334553</v>
+        <v>131.89520093400515</v>
       </c>
       <c r="I6" s="2">
-        <v>101.65217391304348</v>
+        <v>88.518987341772146</v>
       </c>
       <c r="J6" s="2">
         <v>0</v>
@@ -3991,22 +3991,22 @@
         <v>6435</v>
       </c>
       <c r="D7" s="2">
-        <v>9992</v>
+        <v>8264</v>
       </c>
       <c r="E7" s="2">
-        <v>1552.7583527583527</v>
+        <v>1284.2268842268843</v>
       </c>
       <c r="F7" s="2">
-        <v>390.58187134502919</v>
+        <v>393.10175438596491</v>
       </c>
       <c r="G7" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="H7" s="2">
-        <v>118.87274345283497</v>
+        <v>104.49540306462359</v>
       </c>
       <c r="I7" s="2">
-        <v>94.347826086956516</v>
+        <v>82.936708860759495</v>
       </c>
       <c r="J7" s="2">
         <v>0</v>
@@ -4026,22 +4026,22 @@
         <v>5890</v>
       </c>
       <c r="D8" s="2">
-        <v>8169</v>
+        <v>6921</v>
       </c>
       <c r="E8" s="2">
-        <v>1386.9269949066213</v>
+        <v>1175.0424448217318</v>
       </c>
       <c r="F8" s="2">
-        <v>432.47643097643095</v>
+        <v>436.55639730639734</v>
       </c>
       <c r="G8" s="2">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="H8" s="2">
-        <v>131.62326160152244</v>
+        <v>116.04663725866259</v>
       </c>
       <c r="I8" s="2">
-        <v>96.782608695652172</v>
+        <v>85.329113924050631</v>
       </c>
       <c r="J8" s="2">
         <v>0</v>
@@ -4061,22 +4061,22 @@
         <v>4980</v>
       </c>
       <c r="D9" s="2">
-        <v>5597</v>
+        <v>4028</v>
       </c>
       <c r="E9" s="2">
-        <v>1123.8955823293172</v>
+        <v>808.83534136546189</v>
       </c>
       <c r="F9" s="2">
-        <v>382.91336633663371</v>
+        <v>378.31380638063803</v>
       </c>
       <c r="G9" s="2">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="H9" s="2">
-        <v>116.53885062419288</v>
+        <v>100.56442954422023</v>
       </c>
       <c r="I9" s="2">
-        <v>101.34782608695652</v>
+        <v>87.455696202531641</v>
       </c>
       <c r="J9" s="2">
         <v>0</v>
@@ -4096,22 +4096,22 @@
         <v>7020</v>
       </c>
       <c r="D10" s="2">
-        <v>9216</v>
+        <v>6123</v>
       </c>
       <c r="E10" s="2">
-        <v>1312.8205128205129</v>
+        <v>872.22222222222217</v>
       </c>
       <c r="F10" s="2">
-        <v>753.88</v>
+        <v>746.36</v>
       </c>
       <c r="G10" s="2">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="H10" s="2">
-        <v>229.44173913043477</v>
+        <v>198.39949367088607</v>
       </c>
       <c r="I10" s="2">
-        <v>122.04347826086956</v>
+        <v>105.53164556962025</v>
       </c>
       <c r="J10" s="2">
         <v>0</v>
@@ -4131,22 +4131,22 @@
         <v>5320</v>
       </c>
       <c r="D11" s="2">
-        <v>6765</v>
+        <v>5365</v>
       </c>
       <c r="E11" s="2">
-        <v>1271.6165413533834</v>
+        <v>1008.4586466165414</v>
       </c>
       <c r="F11" s="2">
-        <v>367.88395061728392</v>
+        <v>364.10432098765438</v>
       </c>
       <c r="G11" s="2">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H11" s="2">
-        <v>111.96468062265163</v>
+        <v>96.787224566338494</v>
       </c>
       <c r="I11" s="2">
-        <v>88.869565217391298</v>
+        <v>76.822784810126578</v>
       </c>
       <c r="J11" s="2">
         <v>0</v>
@@ -4166,22 +4166,22 @@
         <v>3570</v>
       </c>
       <c r="D12" s="2">
-        <v>4423</v>
+        <v>2889</v>
       </c>
       <c r="E12" s="2">
-        <v>1238.9355742296918</v>
+        <v>809.24369747899163</v>
       </c>
       <c r="F12" s="2">
-        <v>298.62836624775582</v>
+        <v>310.08019150209458</v>
       </c>
       <c r="G12" s="2">
-        <v>339</v>
+        <v>352</v>
       </c>
       <c r="H12" s="2">
-        <v>90.886894075403958</v>
+        <v>82.426380019544126</v>
       </c>
       <c r="I12" s="2">
-        <v>103.17391304347827</v>
+        <v>93.569620253164558</v>
       </c>
       <c r="J12" s="2">
         <v>0</v>
@@ -4201,22 +4201,22 @@
         <v>7356</v>
       </c>
       <c r="D13" s="2">
-        <v>10298</v>
+        <v>7896</v>
       </c>
       <c r="E13" s="2">
-        <v>1399.9456226209898</v>
+        <v>1073.4094616639477</v>
       </c>
       <c r="F13" s="2">
-        <v>507.30662983425418</v>
+        <v>513.34599447513801</v>
       </c>
       <c r="G13" s="2">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="H13" s="2">
-        <v>154.39766994955562</v>
+        <v>136.45906182250505</v>
       </c>
       <c r="I13" s="2">
-        <v>76.695652173913047</v>
+        <v>67.784810126582272</v>
       </c>
       <c r="J13" s="2">
         <v>0</v>
@@ -4231,6 +4231,476 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2695</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3298</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1169.7959989470914</v>
+      </c>
+      <c r="F2" s="2">
+        <v>245.9743386243386</v>
+      </c>
+      <c r="G2" s="2">
+        <v>337</v>
+      </c>
+      <c r="H2" s="2">
+        <v>74.861755233494364</v>
+      </c>
+      <c r="I2" s="2">
+        <v>102.56521739130434</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3100</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4084</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1317.4193548387098</v>
+      </c>
+      <c r="F3" s="2">
+        <v>305.73679417122037</v>
+      </c>
+      <c r="G3" s="2">
+        <v>364</v>
+      </c>
+      <c r="H3" s="2">
+        <v>93.050328660806201</v>
+      </c>
+      <c r="I3" s="2">
+        <v>110.78260869565217</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2800</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3385</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1208.9285714285713</v>
+      </c>
+      <c r="F4" s="2">
+        <v>337.63552188552188</v>
+      </c>
+      <c r="G4" s="2">
+        <v>422</v>
+      </c>
+      <c r="H4" s="2">
+        <v>102.75863709559361</v>
+      </c>
+      <c r="I4" s="2">
+        <v>128.43478260869566</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>69</v>
+      </c>
+      <c r="C5" s="2">
+        <v>6150</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8628</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1402.9268292682927</v>
+      </c>
+      <c r="F5" s="2">
+        <v>456.45124716553283</v>
+      </c>
+      <c r="G5" s="2">
+        <v>317</v>
+      </c>
+      <c r="H5" s="2">
+        <v>138.91994478951</v>
+      </c>
+      <c r="I5" s="2">
+        <v>96.478260869565219</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>71</v>
+      </c>
+      <c r="C6" s="2">
+        <v>6430</v>
+      </c>
+      <c r="D6" s="2">
+        <v>9602</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1493.3125972006221</v>
+      </c>
+      <c r="F6" s="2">
+        <v>497.66720604099248</v>
+      </c>
+      <c r="G6" s="2">
+        <v>334</v>
+      </c>
+      <c r="H6" s="2">
+        <v>151.46393227334553</v>
+      </c>
+      <c r="I6" s="2">
+        <v>101.65217391304348</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>70</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6435</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9992</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1552.7583527583527</v>
+      </c>
+      <c r="F7" s="2">
+        <v>390.58187134502919</v>
+      </c>
+      <c r="G7" s="2">
+        <v>310</v>
+      </c>
+      <c r="H7" s="2">
+        <v>118.87274345283497</v>
+      </c>
+      <c r="I7" s="2">
+        <v>94.347826086956516</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>55</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5890</v>
+      </c>
+      <c r="D8" s="2">
+        <v>8169</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1386.9269949066213</v>
+      </c>
+      <c r="F8" s="2">
+        <v>432.47643097643095</v>
+      </c>
+      <c r="G8" s="2">
+        <v>318</v>
+      </c>
+      <c r="H8" s="2">
+        <v>131.62326160152244</v>
+      </c>
+      <c r="I8" s="2">
+        <v>96.782608695652172</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>48</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4980</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5597</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1123.8955823293172</v>
+      </c>
+      <c r="F9" s="2">
+        <v>382.91336633663371</v>
+      </c>
+      <c r="G9" s="2">
+        <v>333</v>
+      </c>
+      <c r="H9" s="2">
+        <v>116.53885062419288</v>
+      </c>
+      <c r="I9" s="2">
+        <v>101.34782608695652</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>90</v>
+      </c>
+      <c r="C10" s="2">
+        <v>7020</v>
+      </c>
+      <c r="D10" s="2">
+        <v>9216</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1312.8205128205129</v>
+      </c>
+      <c r="F10" s="2">
+        <v>753.88</v>
+      </c>
+      <c r="G10" s="2">
+        <v>401</v>
+      </c>
+      <c r="H10" s="2">
+        <v>229.44173913043477</v>
+      </c>
+      <c r="I10" s="2">
+        <v>122.04347826086956</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>60</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5320</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6765</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1271.6165413533834</v>
+      </c>
+      <c r="F11" s="2">
+        <v>367.88395061728392</v>
+      </c>
+      <c r="G11" s="2">
+        <v>292</v>
+      </c>
+      <c r="H11" s="2">
+        <v>111.96468062265163</v>
+      </c>
+      <c r="I11" s="2">
+        <v>88.869565217391298</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3570</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4423</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1238.9355742296918</v>
+      </c>
+      <c r="F12" s="2">
+        <v>298.62836624775582</v>
+      </c>
+      <c r="G12" s="2">
+        <v>339</v>
+      </c>
+      <c r="H12" s="2">
+        <v>90.886894075403958</v>
+      </c>
+      <c r="I12" s="2">
+        <v>103.17391304347827</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2">
+        <v>98</v>
+      </c>
+      <c r="C13" s="2">
+        <v>7356</v>
+      </c>
+      <c r="D13" s="2">
+        <v>10298</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1399.9456226209898</v>
+      </c>
+      <c r="F13" s="2">
+        <v>507.30662983425418</v>
+      </c>
+      <c r="G13" s="2">
+        <v>252</v>
+      </c>
+      <c r="H13" s="2">
+        <v>154.39766994955562</v>
+      </c>
+      <c r="I13" s="2">
+        <v>76.695652173913047</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
@@ -4706,7 +5176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
@@ -5173,476 +5643,6 @@
       </c>
       <c r="K13" s="2">
         <v>5.88</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2695</v>
-      </c>
-      <c r="D2" s="2">
-        <v>7128</v>
-      </c>
-      <c r="E2" s="2">
-        <v>2644.8979591836733</v>
-      </c>
-      <c r="F2" s="2">
-        <v>228.45687830687828</v>
-      </c>
-      <c r="G2" s="2">
-        <v>313</v>
-      </c>
-      <c r="H2" s="2">
-        <v>94.07047930283224</v>
-      </c>
-      <c r="I2" s="2">
-        <v>128.88235294117646</v>
-      </c>
-      <c r="J2" s="2">
-        <v>75.460000000000008</v>
-      </c>
-      <c r="K2" s="2">
-        <v>28.000000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>40</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3100</v>
-      </c>
-      <c r="D3" s="2">
-        <v>7969</v>
-      </c>
-      <c r="E3" s="2">
-        <v>2570.6451612903224</v>
-      </c>
-      <c r="F3" s="2">
-        <v>284.7383879781421</v>
-      </c>
-      <c r="G3" s="2">
-        <v>339</v>
-      </c>
-      <c r="H3" s="2">
-        <v>117.24521857923499</v>
-      </c>
-      <c r="I3" s="2">
-        <v>139.58823529411765</v>
-      </c>
-      <c r="J3" s="2">
-        <v>62</v>
-      </c>
-      <c r="K3" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>38</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2800</v>
-      </c>
-      <c r="D4" s="2">
-        <v>7302</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2607.8571428571427</v>
-      </c>
-      <c r="F4" s="2">
-        <v>316.03324915824919</v>
-      </c>
-      <c r="G4" s="2">
-        <v>395</v>
-      </c>
-      <c r="H4" s="2">
-        <v>130.13133788869084</v>
-      </c>
-      <c r="I4" s="2">
-        <v>162.64705882352942</v>
-      </c>
-      <c r="J4" s="2">
-        <v>45.36</v>
-      </c>
-      <c r="K4" s="2">
-        <v>16.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>69</v>
-      </c>
-      <c r="C5" s="2">
-        <v>6150</v>
-      </c>
-      <c r="D5" s="2">
-        <v>16389</v>
-      </c>
-      <c r="E5" s="2">
-        <v>2664.8780487804879</v>
-      </c>
-      <c r="F5" s="2">
-        <v>416.13378684807265</v>
-      </c>
-      <c r="G5" s="2">
-        <v>289</v>
-      </c>
-      <c r="H5" s="2">
-        <v>171.34920634920638</v>
-      </c>
-      <c r="I5" s="2">
-        <v>119</v>
-      </c>
-      <c r="J5" s="2">
-        <v>78.289500000000004</v>
-      </c>
-      <c r="K5" s="2">
-        <v>12.73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>71</v>
-      </c>
-      <c r="C6" s="2">
-        <v>6430</v>
-      </c>
-      <c r="D6" s="2">
-        <v>17060</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2653.1881804043546</v>
-      </c>
-      <c r="F6" s="2">
-        <v>449.98651564185542</v>
-      </c>
-      <c r="G6" s="2">
-        <v>302</v>
-      </c>
-      <c r="H6" s="2">
-        <v>185.2885652642934</v>
-      </c>
-      <c r="I6" s="2">
-        <v>124.35294117647059</v>
-      </c>
-      <c r="J6" s="2">
-        <v>125.38500000000001</v>
-      </c>
-      <c r="K6" s="2">
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>70</v>
-      </c>
-      <c r="C7" s="2">
-        <v>6435</v>
-      </c>
-      <c r="D7" s="2">
-        <v>17264</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2682.8282828282827</v>
-      </c>
-      <c r="F7" s="2">
-        <v>355.30350877192984</v>
-      </c>
-      <c r="G7" s="2">
-        <v>282</v>
-      </c>
-      <c r="H7" s="2">
-        <v>146.3014447884417</v>
-      </c>
-      <c r="I7" s="2">
-        <v>116.11764705882354</v>
-      </c>
-      <c r="J7" s="2">
-        <v>123.87375</v>
-      </c>
-      <c r="K7" s="2">
-        <v>19.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
-        <v>55</v>
-      </c>
-      <c r="C8" s="2">
-        <v>5890</v>
-      </c>
-      <c r="D8" s="2">
-        <v>15526</v>
-      </c>
-      <c r="E8" s="2">
-        <v>2635.9932088285227</v>
-      </c>
-      <c r="F8" s="2">
-        <v>403.91666666666674</v>
-      </c>
-      <c r="G8" s="2">
-        <v>297</v>
-      </c>
-      <c r="H8" s="2">
-        <v>166.31862745098042</v>
-      </c>
-      <c r="I8" s="2">
-        <v>122.29411764705883</v>
-      </c>
-      <c r="J8" s="2">
-        <v>97.538399999999996</v>
-      </c>
-      <c r="K8" s="2">
-        <v>16.559999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>48</v>
-      </c>
-      <c r="C9" s="2">
-        <v>4980</v>
-      </c>
-      <c r="D9" s="2">
-        <v>14038</v>
-      </c>
-      <c r="E9" s="2">
-        <v>2818.8755020080321</v>
-      </c>
-      <c r="F9" s="2">
-        <v>344.96699669967001</v>
-      </c>
-      <c r="G9" s="2">
-        <v>300</v>
-      </c>
-      <c r="H9" s="2">
-        <v>142.04523393515825</v>
-      </c>
-      <c r="I9" s="2">
-        <v>123.52941176470588</v>
-      </c>
-      <c r="J9" s="2">
-        <v>104.58</v>
-      </c>
-      <c r="K9" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2">
-        <v>90</v>
-      </c>
-      <c r="C10" s="2">
-        <v>7020</v>
-      </c>
-      <c r="D10" s="2">
-        <v>19024</v>
-      </c>
-      <c r="E10" s="2">
-        <v>2709.9715099715099</v>
-      </c>
-      <c r="F10" s="2">
-        <v>714.4</v>
-      </c>
-      <c r="G10" s="2">
-        <v>380</v>
-      </c>
-      <c r="H10" s="2">
-        <v>294.16470588235296</v>
-      </c>
-      <c r="I10" s="2">
-        <v>156.47058823529412</v>
-      </c>
-      <c r="J10" s="2">
-        <v>132.327</v>
-      </c>
-      <c r="K10" s="2">
-        <v>18.850000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
-        <v>60</v>
-      </c>
-      <c r="C11" s="2">
-        <v>5320</v>
-      </c>
-      <c r="D11" s="2">
-        <v>13836</v>
-      </c>
-      <c r="E11" s="2">
-        <v>2600.7518796992481</v>
-      </c>
-      <c r="F11" s="2">
-        <v>336.38703703703703</v>
-      </c>
-      <c r="G11" s="2">
-        <v>267</v>
-      </c>
-      <c r="H11" s="2">
-        <v>138.51230936819172</v>
-      </c>
-      <c r="I11" s="2">
-        <v>109.94117647058823</v>
-      </c>
-      <c r="J11" s="2">
-        <v>104.27200000000002</v>
-      </c>
-      <c r="K11" s="2">
-        <v>19.600000000000005</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2">
-        <v>45</v>
-      </c>
-      <c r="C12" s="2">
-        <v>3570</v>
-      </c>
-      <c r="D12" s="2">
-        <v>12859</v>
-      </c>
-      <c r="E12" s="2">
-        <v>3601.9607843137255</v>
-      </c>
-      <c r="F12" s="2">
-        <v>233.44105326152004</v>
-      </c>
-      <c r="G12" s="2">
-        <v>265</v>
-      </c>
-      <c r="H12" s="2">
-        <v>96.122786637096496</v>
-      </c>
-      <c r="I12" s="2">
-        <v>109.11764705882354</v>
-      </c>
-      <c r="J12" s="2">
-        <v>74.304000000000002</v>
-      </c>
-      <c r="K12" s="2">
-        <v>19.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="2">
-        <v>98</v>
-      </c>
-      <c r="C13" s="2">
-        <v>7356</v>
-      </c>
-      <c r="D13" s="2">
-        <v>20569</v>
-      </c>
-      <c r="E13" s="2">
-        <v>2796.220772158782</v>
-      </c>
-      <c r="F13" s="2">
-        <v>535.49033149171271</v>
-      </c>
-      <c r="G13" s="2">
-        <v>266</v>
-      </c>
-      <c r="H13" s="2">
-        <v>220.49601884952875</v>
-      </c>
-      <c r="I13" s="2">
-        <v>109.52941176470588</v>
-      </c>
-      <c r="J13" s="2">
-        <v>108.13320000000002</v>
-      </c>
-      <c r="K13" s="2">
-        <v>14.700000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -5706,28 +5706,28 @@
         <v>2695</v>
       </c>
       <c r="D2" s="2">
-        <v>8597</v>
+        <v>7128</v>
       </c>
       <c r="E2" s="2">
-        <v>3189.9814471243044</v>
+        <v>2644.8979591836733</v>
       </c>
       <c r="F2" s="2">
-        <v>226.99708994708996</v>
+        <v>228.45687830687828</v>
       </c>
       <c r="G2" s="2">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="H2" s="2">
-        <v>97.284467120181418</v>
+        <v>94.07047930283224</v>
       </c>
       <c r="I2" s="2">
-        <v>133.28571428571428</v>
+        <v>128.88235294117646</v>
       </c>
       <c r="J2" s="2">
-        <v>107.80000000000001</v>
+        <v>75.460000000000008</v>
       </c>
       <c r="K2" s="2">
-        <v>40</v>
+        <v>28.000000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -5741,28 +5741,28 @@
         <v>3100</v>
       </c>
       <c r="D3" s="2">
-        <v>9723</v>
+        <v>7969</v>
       </c>
       <c r="E3" s="2">
-        <v>3136.4516129032259</v>
+        <v>2570.6451612903224</v>
       </c>
       <c r="F3" s="2">
-        <v>278.85883424408013</v>
+        <v>284.7383879781421</v>
       </c>
       <c r="G3" s="2">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="H3" s="2">
-        <v>119.51092896174863</v>
+        <v>117.24521857923499</v>
       </c>
       <c r="I3" s="2">
-        <v>142.28571428571428</v>
+        <v>139.58823529411765</v>
       </c>
       <c r="J3" s="2">
-        <v>85.25</v>
+        <v>62</v>
       </c>
       <c r="K3" s="2">
-        <v>27.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5776,28 +5776,28 @@
         <v>2800</v>
       </c>
       <c r="D4" s="2">
-        <v>8864</v>
+        <v>7302</v>
       </c>
       <c r="E4" s="2">
-        <v>3165.7142857142858</v>
+        <v>2607.8571428571427</v>
       </c>
       <c r="F4" s="2">
-        <v>311.23274410774411</v>
+        <v>316.03324915824919</v>
       </c>
       <c r="G4" s="2">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="H4" s="2">
-        <v>133.38546176046177</v>
+        <v>130.13133788869084</v>
       </c>
       <c r="I4" s="2">
-        <v>166.71428571428572</v>
+        <v>162.64705882352942</v>
       </c>
       <c r="J4" s="2">
-        <v>75.600000000000009</v>
+        <v>45.36</v>
       </c>
       <c r="K4" s="2">
-        <v>27</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -5811,28 +5811,28 @@
         <v>6150</v>
       </c>
       <c r="D5" s="2">
-        <v>19093</v>
+        <v>16389</v>
       </c>
       <c r="E5" s="2">
-        <v>3104.5528455284552</v>
+        <v>2664.8780487804879</v>
       </c>
       <c r="F5" s="2">
-        <v>411.81405895691614</v>
+        <v>416.13378684807265</v>
       </c>
       <c r="G5" s="2">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="H5" s="2">
-        <v>176.49173955296408</v>
+        <v>171.34920634920638</v>
       </c>
       <c r="I5" s="2">
-        <v>122.57142857142857</v>
+        <v>119</v>
       </c>
       <c r="J5" s="2">
-        <v>132.04050000000001</v>
+        <v>78.289500000000004</v>
       </c>
       <c r="K5" s="2">
-        <v>21.47</v>
+        <v>12.73</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -5846,28 +5846,28 @@
         <v>6430</v>
       </c>
       <c r="D6" s="2">
-        <v>20098</v>
+        <v>17060</v>
       </c>
       <c r="E6" s="2">
-        <v>3125.660964230171</v>
+        <v>2653.1881804043546</v>
       </c>
       <c r="F6" s="2">
-        <v>447.00647249190939</v>
+        <v>449.98651564185542</v>
       </c>
       <c r="G6" s="2">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="H6" s="2">
-        <v>191.57420249653259</v>
+        <v>185.2885652642934</v>
       </c>
       <c r="I6" s="2">
-        <v>128.57142857142858</v>
+        <v>124.35294117647059</v>
       </c>
       <c r="J6" s="2">
-        <v>216.048</v>
+        <v>125.38500000000001</v>
       </c>
       <c r="K6" s="2">
-        <v>33.6</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -5881,28 +5881,28 @@
         <v>6435</v>
       </c>
       <c r="D7" s="2">
-        <v>20264</v>
+        <v>17264</v>
       </c>
       <c r="E7" s="2">
-        <v>3149.0287490287492</v>
+        <v>2682.8282828282827</v>
       </c>
       <c r="F7" s="2">
-        <v>352.78362573099417</v>
+        <v>355.30350877192984</v>
       </c>
       <c r="G7" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="H7" s="2">
-        <v>151.19298245614036</v>
+        <v>146.3014447884417</v>
       </c>
       <c r="I7" s="2">
-        <v>120</v>
+        <v>116.11764705882354</v>
       </c>
       <c r="J7" s="2">
-        <v>168.91874999999999</v>
+        <v>123.87375</v>
       </c>
       <c r="K7" s="2">
-        <v>26.25</v>
+        <v>19.25</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -5916,28 +5916,28 @@
         <v>5890</v>
       </c>
       <c r="D8" s="2">
-        <v>18529</v>
+        <v>15526</v>
       </c>
       <c r="E8" s="2">
-        <v>3145.8404074702885</v>
+        <v>2635.9932088285227</v>
       </c>
       <c r="F8" s="2">
-        <v>395.75673400673395</v>
+        <v>403.91666666666674</v>
       </c>
       <c r="G8" s="2">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="H8" s="2">
-        <v>169.61002886002882</v>
+        <v>166.31862745098042</v>
       </c>
       <c r="I8" s="2">
-        <v>124.71428571428571</v>
+        <v>122.29411764705883</v>
       </c>
       <c r="J8" s="2">
-        <v>155.79050000000001</v>
+        <v>97.538399999999996</v>
       </c>
       <c r="K8" s="2">
-        <v>26.450000000000003</v>
+        <v>16.559999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -5951,28 +5951,28 @@
         <v>4980</v>
       </c>
       <c r="D9" s="2">
-        <v>16199</v>
+        <v>14038</v>
       </c>
       <c r="E9" s="2">
-        <v>3252.8112449799196</v>
+        <v>2818.8755020080321</v>
       </c>
       <c r="F9" s="2">
-        <v>338.06765676567653</v>
+        <v>344.96699669967001</v>
       </c>
       <c r="G9" s="2">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="H9" s="2">
-        <v>144.88613861386136</v>
+        <v>142.04523393515825</v>
       </c>
       <c r="I9" s="2">
-        <v>126</v>
+        <v>123.52941176470588</v>
       </c>
       <c r="J9" s="2">
-        <v>174.3</v>
+        <v>104.58</v>
       </c>
       <c r="K9" s="2">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -5986,28 +5986,28 @@
         <v>7020</v>
       </c>
       <c r="D10" s="2">
-        <v>21526</v>
+        <v>19024</v>
       </c>
       <c r="E10" s="2">
-        <v>3066.3817663817663</v>
+        <v>2709.9715099715099</v>
       </c>
       <c r="F10" s="2">
-        <v>682.44</v>
+        <v>714.4</v>
       </c>
       <c r="G10" s="2">
-        <v>363</v>
+        <v>380</v>
       </c>
       <c r="H10" s="2">
-        <v>292.47428571428571</v>
+        <v>294.16470588235296</v>
       </c>
       <c r="I10" s="2">
-        <v>155.57142857142858</v>
+        <v>156.47058823529412</v>
       </c>
       <c r="J10" s="2">
-        <v>234.11700000000002</v>
+        <v>132.327</v>
       </c>
       <c r="K10" s="2">
-        <v>33.35</v>
+        <v>18.850000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -6021,28 +6021,28 @@
         <v>5320</v>
       </c>
       <c r="D11" s="2">
-        <v>16821</v>
+        <v>13836</v>
       </c>
       <c r="E11" s="2">
-        <v>3161.8421052631579</v>
+        <v>2600.7518796992481</v>
       </c>
       <c r="F11" s="2">
-        <v>332.60740740740744</v>
+        <v>336.38703703703703</v>
       </c>
       <c r="G11" s="2">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="H11" s="2">
-        <v>142.54603174603176</v>
+        <v>138.51230936819172</v>
       </c>
       <c r="I11" s="2">
-        <v>113.14285714285714</v>
+        <v>109.94117647058823</v>
       </c>
       <c r="J11" s="2">
-        <v>171.30400000000003</v>
+        <v>104.27200000000002</v>
       </c>
       <c r="K11" s="2">
-        <v>32.20000000000001</v>
+        <v>19.600000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -6056,28 +6056,28 @@
         <v>3570</v>
       </c>
       <c r="D12" s="2">
-        <v>15123</v>
+        <v>12859</v>
       </c>
       <c r="E12" s="2">
-        <v>4236.134453781513</v>
+        <v>3601.9607843137255</v>
       </c>
       <c r="F12" s="2">
-        <v>223.75104727707961</v>
+        <v>233.44105326152004</v>
       </c>
       <c r="G12" s="2">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="H12" s="2">
-        <v>95.893305975891266</v>
+        <v>96.122786637096496</v>
       </c>
       <c r="I12" s="2">
-        <v>108.85714285714286</v>
+        <v>109.11764705882354</v>
       </c>
       <c r="J12" s="2">
-        <v>83.591999999999999</v>
+        <v>74.304000000000002</v>
       </c>
       <c r="K12" s="2">
-        <v>21.599999999999998</v>
+        <v>19.2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -6091,28 +6091,28 @@
         <v>7356</v>
       </c>
       <c r="D13" s="2">
-        <v>22569</v>
+        <v>20569</v>
       </c>
       <c r="E13" s="2">
-        <v>3068.1076672104405</v>
+        <v>2796.220772158782</v>
       </c>
       <c r="F13" s="2">
-        <v>509.31975138121544</v>
+        <v>535.49033149171271</v>
       </c>
       <c r="G13" s="2">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="H13" s="2">
-        <v>218.27989344909233</v>
+        <v>220.49601884952875</v>
       </c>
       <c r="I13" s="2">
-        <v>98</v>
+        <v>109.52941176470588</v>
       </c>
       <c r="J13" s="2">
-        <v>169.92359999999999</v>
+        <v>108.13320000000002</v>
       </c>
       <c r="K13" s="2">
-        <v>23.1</v>
+        <v>14.700000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>